<commit_message>
parse hojas creadas con datos
</commit_message>
<xml_diff>
--- a/pruebas/src/main/java/practica13/articulos.xlsx
+++ b/pruebas/src/main/java/practica13/articulos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\git\protalento-bootcamp\pruebas\src\main\java\practica13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2A9576-22EA-4364-A78F-C53693CC2324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B26942-A357-4CB1-9C23-6D9A453874CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{8569E67F-19F4-4EED-9D5F-4A0BEE614608}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>titulo</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>cell516</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>mse451</t>
+  </si>
+  <si>
+    <t>teclado</t>
+  </si>
+  <si>
+    <t>tcl4651</t>
   </si>
 </sst>
 </file>
@@ -428,11 +440,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0B2779-DC10-47EC-B0DF-54C8BC9EF603}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -501,6 +511,26 @@
       </c>
       <c r="G3" s="1"/>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -509,7 +539,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EACB846-34E6-4FF5-84C7-6151B5F264AD}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -537,19 +567,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>24500</v>
+        <v>2500</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -557,16 +587,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>1500</v>
+        <v>52000</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -577,42 +607,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>2500</v>
+        <v>2100</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>3</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>52000</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>